<commit_message>
Głodne, bo ciągle jedzą rukole
</commit_message>
<xml_diff>
--- a/pakiety.xlsx
+++ b/pakiety.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JerzyDarzyiOparzy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73323F8F-CCEF-4584-A759-2D0CF786F613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0ADC02-5386-40CB-9AE5-45094735D8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="2500" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +85,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,7 +109,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,16 +168,18 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -437,168 +465,168 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <f>_xlfn.NORM.DIST(186,176,10,TRUE)</f>
         <v>0.84134474606854304</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <f>B2</f>
         <v>0.84134474606854304</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <f>_xlfn.NORM.DIST(166,176,10,TRUE)</f>
         <v>0.15865525393145699</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <f t="shared" ref="C3:C5" si="0">B3</f>
         <v>0.15865525393145699</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <f>1-_xlfn.NORM.DIST(170,176,10,TRUE)</f>
         <v>0.72574688224992645</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <f t="shared" si="0"/>
         <v>0.72574688224992645</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <f>1-_xlfn.NORM.DIST(200,176,10,TRUE)</f>
         <v>8.1975359245961554E-3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>8.1975359245961554E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <f>_xlfn.NORM.DIST(174,176,10,TRUE)-_xlfn.NORM.DIST(168,176,10,TRUE)</f>
         <v>0.20888489197750035</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <f>B6</f>
         <v>0.20888489197750035</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <f>1-_xlfn.NORM.DIST(75,58,10,TRUE)</f>
         <v>4.4565462758543006E-2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <f>B10</f>
         <v>4.4565462758543006E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <f>_xlfn.NORM.DIST(50,58,10,TRUE)</f>
         <v>0.21185539858339661</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <f t="shared" ref="C11:C13" si="1">B11</f>
         <v>0.21185539858339661</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <f>_xlfn.NORM.INV(0.05,58,10)</f>
         <v>41.551463730485274</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="9">
         <f t="shared" si="1"/>
         <v>41.551463730485274</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <f>_xlfn.NORM.INV(0.95,58,10)</f>
         <v>74.448536269514719</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="9">
         <f t="shared" si="1"/>
         <v>74.448536269514719</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="5">
         <f>_xlfn.NORM.DIST(24,36,5,TRUE)</f>
         <v>8.1975359245961311E-3</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <f>B17</f>
         <v>8.1975359245961311E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="10">
         <f>1-_xlfn.NORM.DIST(36,36,5,TRUE)</f>
         <v>0.5</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>